<commit_message>
fixed agriculture mapping to include two more subfuels in 16_other
</commit_message>
<xml_diff>
--- a/config/agriculture_mapping.xlsx
+++ b/config/agriculture_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1338362-22EF-4585-BDB2-A8D2559DD99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D01F840-48EF-4E49-BB41-2D346E9DBBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22050" yWindow="-16395" windowWidth="29040" windowHeight="15840" xr2:uid="{A7B95EFB-A35C-445E-93B3-BE03D78A853B}"/>
+    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{A7B95EFB-A35C-445E-93B3-BE03D78A853B}"/>
   </bookViews>
   <sheets>
     <sheet name="AgricultureMapping" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>Energy Demand (PJ)</t>
   </si>
@@ -153,6 +153,18 @@
   </si>
   <si>
     <t>01_x_thermal_coal</t>
+  </si>
+  <si>
+    <t>16_03_municipal_solid_waste_renewable</t>
+  </si>
+  <si>
+    <t>16_04_municipal_solid_waste_nonrenewable</t>
+  </si>
+  <si>
+    <t>Municipal Solid Waste (Renewable)</t>
+  </si>
+  <si>
+    <t>Municipal Solid Waste (Non-renewable)</t>
   </si>
 </sst>
 </file>
@@ -504,17 +516,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98337923-0FEE-470E-9419-D780835A1568}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -662,34 +674,56 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>35</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bad values of AUS
</commit_message>
<xml_diff>
--- a/config/agriculture_mapping.xlsx
+++ b/config/agriculture_mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D01F840-48EF-4E49-BB41-2D346E9DBBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4C8874-BDB1-48FF-8DD9-669EF3C62D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{A7B95EFB-A35C-445E-93B3-BE03D78A853B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>Energy Demand (PJ)</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>Municipal Solid Waste (Non-renewable)</t>
+  </si>
+  <si>
+    <t>07_02_aviation_gasoline</t>
+  </si>
+  <si>
+    <t>Aviation Gasoline</t>
   </si>
 </sst>
 </file>
@@ -220,9 +226,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -260,7 +266,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -366,7 +372,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -508,7 +514,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -516,7 +522,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98337923-0FEE-470E-9419-D780835A1568}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
@@ -575,155 +581,166 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>26</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>35</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates for pipelines and others
</commit_message>
<xml_diff>
--- a/config/agriculture_mapping.xlsx
+++ b/config/agriculture_mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B545EE73-0214-47C7-971C-F9F9E1BC4DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2D6ACE-AD43-4893-AE1B-23D2DD9CF1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{A7B95EFB-A35C-445E-93B3-BE03D78A853B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
   <si>
     <t>Energy Demand (PJ)</t>
   </si>
@@ -183,6 +183,51 @@
   </si>
   <si>
     <t>Sub-Bituminous Coal</t>
+  </si>
+  <si>
+    <t>02_08_bkb_pb</t>
+  </si>
+  <si>
+    <t>02_01_coke_oven_coke</t>
+  </si>
+  <si>
+    <t>03_peat</t>
+  </si>
+  <si>
+    <t>04_peat_products</t>
+  </si>
+  <si>
+    <t>BKB/PB</t>
+  </si>
+  <si>
+    <t>Peat</t>
+  </si>
+  <si>
+    <t>Peat  Products</t>
+  </si>
+  <si>
+    <t>Crude Oil</t>
+  </si>
+  <si>
+    <t>06_01_crude_oil</t>
+  </si>
+  <si>
+    <t>15_03_charcoal</t>
+  </si>
+  <si>
+    <t>Charcoal</t>
+  </si>
+  <si>
+    <t>Other biomass</t>
+  </si>
+  <si>
+    <t>06_crude_oil_and_ngl</t>
+  </si>
+  <si>
+    <t>Industrial Waste</t>
+  </si>
+  <si>
+    <t>16_02_industrial_waste</t>
   </si>
 </sst>
 </file>
@@ -534,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98337923-0FEE-470E-9419-D780835A1568}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,182 +655,259 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>26</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B29" t="s">
         <v>35</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C29" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed heat output mapping/calculations
</commit_message>
<xml_diff>
--- a/config/agriculture_mapping.xlsx
+++ b/config/agriculture_mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2D6ACE-AD43-4893-AE1B-23D2DD9CF1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B210332-7886-423B-B5AE-BD2CBFE1F804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{A7B95EFB-A35C-445E-93B3-BE03D78A853B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
   <si>
     <t>Energy Demand (PJ)</t>
   </si>
@@ -228,6 +228,12 @@
   </si>
   <si>
     <t>16_02_industrial_waste</t>
+  </si>
+  <si>
+    <t>06_02_natural_gas_liquids</t>
+  </si>
+  <si>
+    <t>Natural Gas Liquids</t>
   </si>
 </sst>
 </file>
@@ -579,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98337923-0FEE-470E-9419-D780835A1568}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,128 +710,128 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
@@ -836,78 +842,89 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>26</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>35</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>